<commit_message>
[2019. 08. 15] 1. 광복절!!! 2. Document Index 수정 > Swagger 오타 수정 3. Document Index 삭제 후 목록 반환 시 last-page 설정 4. Excel 업로드 시 header 값 변경 (Excel에서 header 없이 작성) / header 값 변경에 따른 documentInfo 저장 로직 수정
</commit_message>
<xml_diff>
--- a/upload/test.xlsx
+++ b/upload/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iseongmin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21819894-FEF9-CF48-A32D-6EA69769DEFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8C6D80-F039-774D-B1EC-BD39E683B8B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{4095E49F-4A7B-BA41-BD21-08796E1061B1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>VP-NCC-R-001-001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,18 +66,6 @@
   </si>
   <si>
     <t>Welding Procedure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>plan</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -460,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{189D3A86-E49E-2848-994B-D1ECDF751982}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -475,68 +463,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>43718</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43718</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43718</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
-        <v>43718</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[2019. 08. 17] 1. Document Index > Document Info 개별 추가, Document Index 검색 추가
</commit_message>
<xml_diff>
--- a/upload/test.xlsx
+++ b/upload/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iseongmin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8C6D80-F039-774D-B1EC-BD39E683B8B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B365ACD3-C15F-F64B-B20C-5AB42817CF2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{4095E49F-4A7B-BA41-BD21-08796E1061B1}"/>
   </bookViews>
@@ -33,26 +33,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>VP-NCC-R-001-001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Vendor Print Index &amp; Schedule</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VP-NCC-R-001-002</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-001-003</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-001-004</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-001-005</t>
-  </si>
-  <si>
     <t>Sub-Vendor List</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,6 +63,22 @@
   <si>
     <t>2019.09.13</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VP-NCC-R-004-001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VP-NCC-R-004-002</t>
+  </si>
+  <si>
+    <t>VP-NCC-R-004-003</t>
+  </si>
+  <si>
+    <t>VP-NCC-R-004-004</t>
+  </si>
+  <si>
+    <t>VP-NCC-R-004-005</t>
   </si>
 </sst>
 </file>
@@ -463,10 +463,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="2">
         <v>43718</v>
@@ -474,21 +474,21 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>43718</v>
@@ -496,24 +496,24 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[2019. 09. 23] 1. Project 스키마 추가 2. Project 목록, 조회, 추가 완료
</commit_message>
<xml_diff>
--- a/upload/test.xlsx
+++ b/upload/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iseongmin/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iseongmin/Downloads/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B365ACD3-C15F-F64B-B20C-5AB42817CF2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5209E3D5-8778-DE4A-ABBB-F7F18731D386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{4095E49F-4A7B-BA41-BD21-08796E1061B1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{4095E49F-4A7B-BA41-BD21-08796E1061B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,20 +65,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VP-NCC-R-004-001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VP-NCC-R-004-002</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-004-003</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-004-004</t>
-  </si>
-  <si>
-    <t>VP-NCC-R-004-005</t>
+    <t>VP-NCC-S-013-001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VP-NCC-S-013-002</t>
+  </si>
+  <si>
+    <t>VP-NCC-S-013-003</t>
+  </si>
+  <si>
+    <t>VP-NCC-S-013-004</t>
+  </si>
+  <si>
+    <t>VP-NCC-S-013-005</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>

</xml_diff>